<commit_message>
Update Cópia de brimunobiogico-sct_eng-10_07_23 Revisãomapeamento09082023.xlsx
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Imunizacao/Mapeamento BRImunobiológico/Cópia de brimunobiogico-sct_eng-10_07_23 Revisãomapeamento09082023.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Imunizacao/Mapeamento BRImunobiológico/Cópia de brimunobiogico-sct_eng-10_07_23 Revisãomapeamento09082023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Imunizacao/Mapeamento BRImunobiológico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EACEB221-8339-0841-83EB-FF83016F77D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BAEF12-BA65-934B-8276-83EEAC9E8670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapping!$A$3:$J$78</definedName>
   </definedNames>
-  <calcPr calcId="162913" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -791,19 +802,6 @@
     <t>OBSERV</t>
   </si>
   <si>
-    <r>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="4"/>
-        <rFont val="Calibri (Corpo)"/>
-      </rPr>
-      <t>oro é Imunoglobulina (substância) para tratar pacientes já enfermos, vacina é toxina inativada</t>
-    </r>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -956,12 +954,25 @@
     <t xml:space="preserve">Quadrivalente? CDC’s Advisory Committee on Immunization Practices (ACIP) recently recommended preferentially using Fluzone High-Dose Quadrivalent (inactivated influenza vaccine [IIV4-HD]), Flublok Quadrivalent (recombinant influenza vaccine [RIV4]), or Fluad Quadrivalent (adjuvanted inactivated influenza vaccine quadrivalent [aIIV4]) for this age group. If high-dose or adjuvanted vaccines aren’t available, a standard seasonal influenza vaccine is recommended for older adults, the ACIP statement noted.
 </t>
   </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corpo)"/>
+      </rPr>
+      <t>oro é Imunoglobulina (substância) para tratar pacientes já enfermos, vacina é toxina inativada</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1047,11 +1058,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="4"/>
-      <name val="Calibri (Corpo)"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Corpo)"/>
     </font>
@@ -1070,7 +1076,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,6 +1110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1355,24 +1367,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,29 +1380,50 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1722,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1046725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C41" zoomScale="131" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="131" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1766,7 +1781,7 @@
       <c r="K1" s="48" t="s">
         <v>234</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="54" t="s">
         <v>235</v>
       </c>
       <c r="M1" s="48" t="s">
@@ -1799,7 +1814,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="7"/>
       <c r="K2" s="49"/>
-      <c r="L2" s="61"/>
+      <c r="L2" s="55"/>
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1833,7 +1848,7 @@
         <v>17</v>
       </c>
       <c r="K3" s="49"/>
-      <c r="L3" s="61"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -1865,7 +1880,7 @@
         <v>23</v>
       </c>
       <c r="K4" s="49"/>
-      <c r="L4" s="61"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -1899,7 +1914,7 @@
         <v>23</v>
       </c>
       <c r="K5" s="49"/>
-      <c r="L5" s="61"/>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -1933,7 +1948,7 @@
         <v>23</v>
       </c>
       <c r="K6" s="49"/>
-      <c r="L6" s="61"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:15" s="46" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
@@ -1970,14 +1985,14 @@
         <v>240</v>
       </c>
       <c r="L7" s="47"/>
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="71" t="s">
         <v>244</v>
       </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="O7" s="65" t="s">
-        <v>246</v>
+      <c r="O7" s="72" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2012,7 +2027,7 @@
         <v>23</v>
       </c>
       <c r="K8" s="49"/>
-      <c r="L8" s="61"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
@@ -2046,7 +2061,7 @@
         <v>23</v>
       </c>
       <c r="K9" s="49"/>
-      <c r="L9" s="61"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
@@ -2074,7 +2089,7 @@
         <v>23</v>
       </c>
       <c r="K10" s="49"/>
-      <c r="L10" s="61"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
@@ -2108,7 +2123,7 @@
         <v>23</v>
       </c>
       <c r="K11" s="49"/>
-      <c r="L11" s="61"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
@@ -2140,7 +2155,7 @@
         <v>23</v>
       </c>
       <c r="K12" s="49"/>
-      <c r="L12" s="61"/>
+      <c r="L12" s="55"/>
     </row>
     <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -2176,11 +2191,11 @@
       <c r="K13" s="49" t="s">
         <v>229</v>
       </c>
-      <c r="L13" s="61" t="s">
+      <c r="L13" s="55" t="s">
         <v>72</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2217,9 +2232,9 @@
       <c r="K14" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="55"/>
     </row>
     <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
@@ -2249,9 +2264,9 @@
       <c r="K15" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="61"/>
+      <c r="L15" s="55"/>
       <c r="O15" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2288,11 +2303,11 @@
       <c r="K16" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="L16" s="61" t="s">
+      <c r="L16" s="55" t="s">
         <v>242</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2327,10 +2342,10 @@
         <v>23</v>
       </c>
       <c r="K17" s="49"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
     </row>
     <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
@@ -2364,7 +2379,7 @@
         <v>23</v>
       </c>
       <c r="K18" s="50"/>
-      <c r="L18" s="62"/>
+      <c r="L18" s="56"/>
     </row>
     <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
@@ -2398,8 +2413,8 @@
         <v>23</v>
       </c>
       <c r="K19" s="49"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="70">
+      <c r="L19" s="55"/>
+      <c r="M19" s="63">
         <v>871739009</v>
       </c>
     </row>
@@ -2437,11 +2452,11 @@
       <c r="K20" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="L20" s="61" t="s">
+      <c r="L20" s="55" t="s">
         <v>80</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="225" x14ac:dyDescent="0.2">
@@ -2478,17 +2493,17 @@
       <c r="K21" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="L21" s="61" t="s">
+      <c r="L21" s="55" t="s">
         <v>237</v>
       </c>
       <c r="M21" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="N21" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="O21" s="55" t="s">
         <v>250</v>
-      </c>
-      <c r="N21" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="O21" s="61" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
@@ -2517,23 +2532,23 @@
         <v>87</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="J22" s="68" t="s">
+        <v>252</v>
+      </c>
+      <c r="J22" s="61" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="L22" s="61"/>
-      <c r="M22" s="67" t="s">
-        <v>258</v>
-      </c>
-      <c r="N22" s="67" t="s">
-        <v>252</v>
-      </c>
-      <c r="O22" s="67" t="s">
-        <v>254</v>
+      <c r="L22" s="55"/>
+      <c r="M22" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="N22" s="60" t="s">
+        <v>251</v>
+      </c>
+      <c r="O22" s="60" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2570,12 +2585,12 @@
       <c r="K23" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="L23" s="61" t="s">
+      <c r="L23" s="55" t="s">
         <v>93</v>
       </c>
       <c r="M23" s="39"/>
       <c r="O23" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2610,7 +2625,7 @@
         <v>84</v>
       </c>
       <c r="K24" s="49"/>
-      <c r="L24" s="61"/>
+      <c r="L24" s="55"/>
     </row>
     <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
@@ -2627,7 +2642,7 @@
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="69" t="s">
+      <c r="G25" s="62" t="s">
         <v>99</v>
       </c>
       <c r="H25" s="40" t="s">
@@ -2642,11 +2657,11 @@
       <c r="K25" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="55" t="s">
         <v>102</v>
       </c>
       <c r="O25" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2683,11 +2698,11 @@
       <c r="K26" s="49" t="s">
         <v>239</v>
       </c>
-      <c r="L26" s="61" t="s">
+      <c r="L26" s="55" t="s">
         <v>232</v>
       </c>
       <c r="O26" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="60" x14ac:dyDescent="0.2">
@@ -2722,7 +2737,7 @@
         <v>23</v>
       </c>
       <c r="K27" s="49"/>
-      <c r="L27" s="61"/>
+      <c r="L27" s="55"/>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
@@ -2756,7 +2771,7 @@
         <v>23</v>
       </c>
       <c r="K28" s="49"/>
-      <c r="L28" s="61"/>
+      <c r="L28" s="55"/>
     </row>
     <row r="29" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
@@ -2790,7 +2805,7 @@
         <v>23</v>
       </c>
       <c r="K29" s="49"/>
-      <c r="L29" s="61"/>
+      <c r="L29" s="55"/>
     </row>
     <row r="30" spans="1:15" ht="75" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
@@ -2822,7 +2837,7 @@
         <v>23</v>
       </c>
       <c r="K30" s="49"/>
-      <c r="L30" s="61"/>
+      <c r="L30" s="55"/>
     </row>
     <row r="31" spans="1:15" ht="90" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
@@ -2858,11 +2873,11 @@
       <c r="K31" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="L31" s="61" t="s">
+      <c r="L31" s="55" t="s">
         <v>121</v>
       </c>
       <c r="O31" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -2897,7 +2912,7 @@
         <v>84</v>
       </c>
       <c r="K32" s="49"/>
-      <c r="L32" s="61"/>
+      <c r="L32" s="55"/>
     </row>
     <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
@@ -2931,7 +2946,7 @@
         <v>84</v>
       </c>
       <c r="K33" s="49"/>
-      <c r="L33" s="61"/>
+      <c r="L33" s="55"/>
     </row>
     <row r="34" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
@@ -2965,7 +2980,7 @@
         <v>23</v>
       </c>
       <c r="K34" s="49"/>
-      <c r="L34" s="61"/>
+      <c r="L34" s="55"/>
     </row>
     <row r="35" spans="1:15" ht="240" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
@@ -2992,19 +3007,19 @@
       <c r="H35" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I35" s="71" t="s">
-        <v>266</v>
+      <c r="I35" s="64" t="s">
+        <v>265</v>
       </c>
       <c r="J35" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K35" s="49"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61" t="s">
+      <c r="L35" s="55"/>
+      <c r="M35" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="N35" s="55" t="s">
         <v>264</v>
-      </c>
-      <c r="N35" s="61" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="210" x14ac:dyDescent="0.2">
@@ -3041,14 +3056,14 @@
       <c r="K36" s="49" t="s">
         <v>238</v>
       </c>
-      <c r="L36" s="61" t="s">
+      <c r="L36" s="55" t="s">
         <v>237</v>
       </c>
-      <c r="M36" s="61" t="s">
+      <c r="M36" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="N36" s="55" t="s">
         <v>259</v>
-      </c>
-      <c r="N36" s="61" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="120" x14ac:dyDescent="0.2">
@@ -3077,18 +3092,18 @@
         <v>96</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="J37" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="J37" s="61" t="s">
         <v>23</v>
       </c>
       <c r="K37" s="49"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="N37" s="61" t="s">
-        <v>267</v>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="N37" s="55" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="60" x14ac:dyDescent="0.2">
@@ -3117,7 +3132,7 @@
         <v>140</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>23</v>
@@ -3125,11 +3140,11 @@
       <c r="K38" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="L38" s="61" t="s">
+      <c r="L38" s="55" t="s">
         <v>230</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="240" x14ac:dyDescent="0.2">
@@ -3164,12 +3179,12 @@
         <v>84</v>
       </c>
       <c r="K39" s="49"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61" t="s">
+      <c r="L39" s="55"/>
+      <c r="M39" s="55" t="s">
+        <v>269</v>
+      </c>
+      <c r="N39" s="55" t="s">
         <v>270</v>
-      </c>
-      <c r="N39" s="61" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="314" x14ac:dyDescent="0.2">
@@ -3206,7 +3221,7 @@
       <c r="M40" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="N40" s="61" t="s">
+      <c r="N40" s="55" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3242,7 +3257,7 @@
         <v>23</v>
       </c>
       <c r="K41" s="49"/>
-      <c r="L41" s="61"/>
+      <c r="L41" s="55"/>
     </row>
     <row r="42" spans="1:15" ht="75" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
@@ -3269,8 +3284,8 @@
       <c r="H42" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="I42" s="71" t="s">
-        <v>272</v>
+      <c r="I42" s="64" t="s">
+        <v>271</v>
       </c>
       <c r="J42" s="11" t="s">
         <v>84</v>
@@ -3278,11 +3293,11 @@
       <c r="K42" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="L42" s="61" t="s">
+      <c r="L42" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="N42" s="61" t="s">
-        <v>247</v>
+      <c r="N42" s="55" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3319,11 +3334,11 @@
       <c r="K43" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="L43" s="61" t="s">
+      <c r="L43" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="N43" s="61" t="s">
-        <v>247</v>
+      <c r="N43" s="55" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
@@ -3358,9 +3373,9 @@
         <v>84</v>
       </c>
       <c r="K44" s="49"/>
-      <c r="L44" s="61"/>
-      <c r="O44" s="61" t="s">
-        <v>277</v>
+      <c r="L44" s="55"/>
+      <c r="O44" s="55" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3395,7 +3410,7 @@
         <v>84</v>
       </c>
       <c r="K45" s="49"/>
-      <c r="L45" s="61"/>
+      <c r="L45" s="55"/>
     </row>
     <row r="46" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
@@ -3431,9 +3446,9 @@
       <c r="K46" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="L46" s="61"/>
+      <c r="L46" s="55"/>
       <c r="M46" s="49"/>
-      <c r="N46" s="61"/>
+      <c r="N46" s="55"/>
       <c r="O46" s="12"/>
     </row>
     <row r="47" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3468,7 +3483,7 @@
         <v>84</v>
       </c>
       <c r="K47" s="49"/>
-      <c r="L47" s="61"/>
+      <c r="L47" s="55"/>
     </row>
     <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
@@ -3502,7 +3517,7 @@
         <v>23</v>
       </c>
       <c r="K48" s="49"/>
-      <c r="L48" s="61"/>
+      <c r="L48" s="55"/>
     </row>
     <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
@@ -3538,11 +3553,11 @@
       <c r="K49" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="L49" s="61" t="s">
+      <c r="L49" s="55" t="s">
         <v>220</v>
       </c>
       <c r="O49" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3579,27 +3594,27 @@
       <c r="K50" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="L50" s="61" t="s">
+      <c r="L50" s="55" t="s">
         <v>221</v>
       </c>
       <c r="O50" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="56">
+      <c r="A51" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="67">
         <v>70</v>
       </c>
-      <c r="C51" s="54" t="s">
+      <c r="C51" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="D51" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="58" t="s">
+      <c r="D51" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="69" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="8" t="s">
@@ -3618,14 +3633,14 @@
         <v>56</v>
       </c>
       <c r="K51" s="49"/>
-      <c r="L51" s="61"/>
+      <c r="L51" s="55"/>
     </row>
     <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="55"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="59"/>
+      <c r="A52" s="66"/>
+      <c r="B52" s="68"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="70"/>
       <c r="F52" s="8" t="s">
         <v>7</v>
       </c>
@@ -3642,7 +3657,7 @@
         <v>56</v>
       </c>
       <c r="K52" s="49"/>
-      <c r="L52" s="61"/>
+      <c r="L52" s="55"/>
     </row>
     <row r="53" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
@@ -3676,7 +3691,7 @@
         <v>23</v>
       </c>
       <c r="K53" s="49"/>
-      <c r="L53" s="61"/>
+      <c r="L53" s="55"/>
     </row>
     <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
@@ -3710,7 +3725,7 @@
         <v>56</v>
       </c>
       <c r="K54" s="49"/>
-      <c r="L54" s="61"/>
+      <c r="L54" s="55"/>
     </row>
     <row r="55" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
@@ -3746,11 +3761,11 @@
       <c r="K55" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="L55" s="61" t="s">
+      <c r="L55" s="55" t="s">
         <v>230</v>
       </c>
       <c r="O55" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3785,7 +3800,7 @@
         <v>23</v>
       </c>
       <c r="K56" s="49"/>
-      <c r="L56" s="61"/>
+      <c r="L56" s="55"/>
     </row>
     <row r="57" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
@@ -3821,11 +3836,11 @@
       <c r="K57" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="L57" s="61" t="s">
+      <c r="L57" s="55" t="s">
         <v>233</v>
       </c>
       <c r="O57" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3853,12 +3868,12 @@
       <c r="K58" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="L58" s="61" t="s">
+      <c r="L58" s="55" t="s">
         <v>93</v>
       </c>
       <c r="M58" s="39"/>
       <c r="O58" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
@@ -3895,15 +3910,15 @@
       <c r="K59" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="L59" s="61"/>
+      <c r="L59" s="55"/>
       <c r="M59" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="N59" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="O59" s="49" t="s">
         <v>256</v>
-      </c>
-      <c r="N59" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="O59" s="49" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -3938,7 +3953,7 @@
         <v>23</v>
       </c>
       <c r="K60" s="49"/>
-      <c r="L60" s="61"/>
+      <c r="L60" s="55"/>
     </row>
     <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
@@ -3972,7 +3987,7 @@
         <v>23</v>
       </c>
       <c r="K61" s="49"/>
-      <c r="L61" s="61"/>
+      <c r="L61" s="55"/>
     </row>
     <row r="62" spans="1:15" ht="105" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
@@ -4000,18 +4015,18 @@
         <v>96</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J62" s="11" t="s">
         <v>84</v>
       </c>
       <c r="K62" s="49"/>
-      <c r="L62" s="61"/>
-      <c r="M62" s="61">
+      <c r="L62" s="55"/>
+      <c r="M62" s="55">
         <v>865997008</v>
       </c>
-      <c r="N62" s="61" t="s">
-        <v>273</v>
+      <c r="N62" s="55" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -4046,7 +4061,7 @@
         <v>23</v>
       </c>
       <c r="K63" s="49"/>
-      <c r="L63" s="61"/>
+      <c r="L63" s="55"/>
     </row>
     <row r="64" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
@@ -4080,7 +4095,7 @@
         <v>84</v>
       </c>
       <c r="K64" s="49"/>
-      <c r="L64" s="61"/>
+      <c r="L64" s="55"/>
     </row>
     <row r="65" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
@@ -4114,7 +4129,7 @@
         <v>84</v>
       </c>
       <c r="K65" s="49"/>
-      <c r="L65" s="61"/>
+      <c r="L65" s="55"/>
     </row>
     <row r="66" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
@@ -4148,7 +4163,7 @@
         <v>84</v>
       </c>
       <c r="K66" s="49"/>
-      <c r="L66" s="61"/>
+      <c r="L66" s="55"/>
     </row>
     <row r="67" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
@@ -4182,7 +4197,7 @@
         <v>84</v>
       </c>
       <c r="K67" s="49"/>
-      <c r="L67" s="61"/>
+      <c r="L67" s="55"/>
     </row>
     <row r="68" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
@@ -4216,7 +4231,7 @@
         <v>84</v>
       </c>
       <c r="K68" s="49"/>
-      <c r="L68" s="61"/>
+      <c r="L68" s="55"/>
     </row>
     <row r="69" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
@@ -4252,11 +4267,11 @@
       <c r="K69" s="49" t="s">
         <v>239</v>
       </c>
-      <c r="L69" s="61" t="s">
+      <c r="L69" s="55" t="s">
         <v>232</v>
       </c>
       <c r="O69" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="45" x14ac:dyDescent="0.2">
@@ -4293,11 +4308,11 @@
       <c r="K70" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="L70" s="63" t="s">
+      <c r="L70" s="57" t="s">
         <v>223</v>
       </c>
       <c r="O70" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="60" x14ac:dyDescent="0.2">
@@ -4332,7 +4347,7 @@
         <v>84</v>
       </c>
       <c r="K71" s="51"/>
-      <c r="L71" s="64"/>
+      <c r="L71" s="58"/>
     </row>
     <row r="72" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
@@ -4366,7 +4381,7 @@
         <v>84</v>
       </c>
       <c r="K72" s="51"/>
-      <c r="L72" s="64"/>
+      <c r="L72" s="58"/>
     </row>
     <row r="73" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
@@ -4400,7 +4415,7 @@
         <v>84</v>
       </c>
       <c r="K73" s="51"/>
-      <c r="L73" s="64"/>
+      <c r="L73" s="58"/>
     </row>
     <row r="74" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
@@ -4434,7 +4449,7 @@
         <v>84</v>
       </c>
       <c r="K74" s="51"/>
-      <c r="L74" s="64"/>
+      <c r="L74" s="58"/>
     </row>
     <row r="75" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
@@ -4468,7 +4483,7 @@
         <v>84</v>
       </c>
       <c r="K75" s="51"/>
-      <c r="L75" s="64"/>
+      <c r="L75" s="58"/>
     </row>
     <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
@@ -4502,7 +4517,7 @@
         <v>84</v>
       </c>
       <c r="K76" s="51"/>
-      <c r="L76" s="64"/>
+      <c r="L76" s="58"/>
     </row>
     <row r="77" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
@@ -4536,7 +4551,7 @@
         <v>84</v>
       </c>
       <c r="K77" s="51"/>
-      <c r="L77" s="64"/>
+      <c r="L77" s="58"/>
     </row>
     <row r="78" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
@@ -4570,9 +4585,9 @@
         <v>23</v>
       </c>
       <c r="K78" s="50"/>
-      <c r="L78" s="62"/>
+      <c r="L78" s="56"/>
       <c r="O78" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
@@ -4606,12 +4621,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4830,15 +4842,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B595ECDB-A699-4CE2-BEFD-D76F82876E3D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2473D3FE-6936-4D3A-85B9-D91536E4F0AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b0ada803-87a5-4f80-bf3c-49fd012dc2db"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="8c04557f-fd53-4c74-80a8-0d8bfa82ceea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4863,18 +4887,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2473D3FE-6936-4D3A-85B9-D91536E4F0AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B595ECDB-A699-4CE2-BEFD-D76F82876E3D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b0ada803-87a5-4f80-bf3c-49fd012dc2db"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8c04557f-fd53-4c74-80a8-0d8bfa82ceea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>